<commit_message>
negative sample + compare framework + compare DS weight
</commit_message>
<xml_diff>
--- a/evaluations/evaluation_all.xlsx
+++ b/evaluations/evaluation_all.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACA8956-5489-4901-A949-B6B2967E8E64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED1E221-F719-4CC4-BC6A-954D5C64A721}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>P@1</t>
   </si>
@@ -105,10 +105,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>generator1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RoBERTa_DGen_model4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -129,27 +125,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BATCH_SIZE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPOCH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LEARNING_RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAX_LENGTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BERT_model1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SciBERT_model1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SciBERT_DGen_neg_model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SciBERT_CLOTH&amp;DGen_neg_model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -157,10 +145,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,13 +207,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -349,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -415,9 +393,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -425,17 +400,6 @@
     <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -443,7 +407,7 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="19">
     <dxf>
       <font>
         <b val="0"/>
@@ -778,66 +742,6 @@
         <charset val="136"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -967,20 +871,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B9FD7945-2DBD-4D1D-89A7-357D6BC32B92}" name="表格2" displayName="表格2" ref="A2:K26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A2:K26" xr:uid="{C751FB98-FFA8-4E36-A938-9D2D2B10C92F}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{39C2CA48-6F9D-4AA1-A8A7-EBC45FC3EBF7}" name="models" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{575579F2-5151-4D34-A661-861B38B56F85}" name="P@1" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{AD6CB662-C0FF-4BD1-9857-B94030501B28}" name="P@3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{362F5AF3-576A-4ACF-B3BE-AD79B3DF0FC8}" name="R@3" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{ACC81680-F827-4C06-83A4-D97A94EA14AB}" name="F1@3" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{DC454E98-3A64-4075-B3EA-CF92952FF2CF}" name="MRR" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{F61F6C8D-8040-49CB-B130-5EC8A135200A}" name="NDCG@10" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{3A9C7A93-E32B-40D6-B7C6-43B74CB87B15}" name="BATCH_SIZE" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{71D90EEB-5DFE-4ACB-A2BC-9B87F25900E4}" name="EPOCH" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{0B5B748D-F1C5-49DA-89CB-672AB77BF78C}" name="LEARNING_RATE" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{E2271A6C-BB5B-4213-ACAA-93D960DD9B24}" name="MAX_LENGTH" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B9FD7945-2DBD-4D1D-89A7-357D6BC32B92}" name="表格2" displayName="表格2" ref="A1:G27" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:G27" xr:uid="{C751FB98-FFA8-4E36-A938-9D2D2B10C92F}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{39C2CA48-6F9D-4AA1-A8A7-EBC45FC3EBF7}" name="models" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{575579F2-5151-4D34-A661-861B38B56F85}" name="P@1" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{AD6CB662-C0FF-4BD1-9857-B94030501B28}" name="P@3" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{362F5AF3-576A-4ACF-B3BE-AD79B3DF0FC8}" name="R@3" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{ACC81680-F827-4C06-83A4-D97A94EA14AB}" name="F1@3" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{DC454E98-3A64-4075-B3EA-CF92952FF2CF}" name="MRR" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{F61F6C8D-8040-49CB-B130-5EC8A135200A}" name="NDCG@10" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1265,788 +1165,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.75" style="3" customWidth="1"/>
+    <col min="1" max="1" width="39.625" style="3" customWidth="1"/>
     <col min="2" max="6" width="12.625" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.625" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="3"/>
+    <col min="8" max="10" width="10.625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6">
+        <v>9.31</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5.81</v>
+      </c>
+      <c r="D2" s="6">
+        <v>12.98</v>
+      </c>
+      <c r="E2" s="6">
+        <v>7.71</v>
+      </c>
+      <c r="F2" s="6">
+        <v>14.34</v>
+      </c>
+      <c r="G2" s="6">
+        <v>14.94</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7">
+        <v>10.85</v>
+      </c>
+      <c r="C3" s="7">
+        <v>6.72</v>
+      </c>
+      <c r="D3" s="7">
+        <v>15.88</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9.19</v>
+      </c>
+      <c r="F3" s="7">
+        <v>17.510000000000002</v>
+      </c>
+      <c r="G3" s="6">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5.01</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3.98</v>
+      </c>
+      <c r="D4" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>5.59</v>
+      </c>
+      <c r="F4" s="7">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="G4" s="6">
+        <v>11.6</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2.3166023166023102</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2.0592020592020499</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2.0592020592020499</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2.0592020592020499</v>
+      </c>
+      <c r="F5" s="9">
+        <v>4.5875467304038704</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6.3742694961931496</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4.6332046332046302</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4.3758043758043703</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4.3758043758043703</v>
+      </c>
+      <c r="E6" s="9">
+        <v>4.3758043758043703</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9.1829073971931106</v>
+      </c>
+      <c r="G6" s="9">
+        <v>13.7623852619798</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="C7" s="10">
+        <v>6.9498069498069501</v>
+      </c>
+      <c r="D7" s="10">
+        <v>6.9498069498069501</v>
+      </c>
+      <c r="E7" s="10">
+        <v>6.9498069498069501</v>
+      </c>
+      <c r="F7" s="10">
+        <v>15.4283875712447</v>
+      </c>
+      <c r="G7" s="10">
+        <v>22.680937559473801</v>
+      </c>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10">
+        <v>10.8108108108108</v>
+      </c>
+      <c r="C8" s="10">
+        <v>7.3359073359073301</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7.3359073359073301</v>
+      </c>
+      <c r="E8" s="10">
+        <v>7.3359073359073301</v>
+      </c>
+      <c r="F8" s="10">
+        <v>17.481154624011701</v>
+      </c>
+      <c r="G8" s="10">
+        <v>23.049457237024701</v>
+      </c>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1.54440154440154</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2.57400257400257</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2.57400257400257</v>
+      </c>
+      <c r="E9" s="12">
+        <v>2.57400257400257</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5.2253784396641496</v>
+      </c>
+      <c r="G9" s="12">
+        <v>8.5634595960399391</v>
+      </c>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="12">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="C10" s="12">
+        <v>5.0193050193050199</v>
+      </c>
+      <c r="D10" s="12">
+        <v>5.0193050193050199</v>
+      </c>
+      <c r="E10" s="12">
+        <v>5.0193050193050199</v>
+      </c>
+      <c r="F10" s="12">
+        <v>11.9784580498866</v>
+      </c>
+      <c r="G10" s="12">
+        <v>15.6911707723312</v>
+      </c>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="12">
+        <v>15.444015444015401</v>
+      </c>
+      <c r="C11" s="12">
+        <v>10.8108108108108</v>
+      </c>
+      <c r="D11" s="12">
+        <v>10.8108108108108</v>
+      </c>
+      <c r="E11" s="12">
+        <v>10.8108108108108</v>
+      </c>
+      <c r="F11" s="12">
+        <v>24.998467855610699</v>
+      </c>
+      <c r="G11" s="20">
+        <v>32.401329519520097</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="20">
+        <v>17.760617760617698</v>
+      </c>
+      <c r="C12" s="20">
+        <v>12.226512226512201</v>
+      </c>
+      <c r="D12" s="20">
+        <v>12.226512226512201</v>
+      </c>
+      <c r="E12" s="20">
+        <v>12.226512226512201</v>
+      </c>
+      <c r="F12" s="20">
+        <v>26.0492124777839</v>
+      </c>
+      <c r="G12" s="12">
+        <v>31.838706064182698</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="34">
+        <v>1.54440154440154</v>
+      </c>
+      <c r="C13" s="34">
+        <v>4.1184041184041096</v>
+      </c>
+      <c r="D13" s="34">
+        <v>4.1184041184041096</v>
+      </c>
+      <c r="E13" s="34">
+        <v>4.1184041184041096</v>
+      </c>
+      <c r="F13" s="34">
+        <v>8.8452227737942</v>
+      </c>
+      <c r="G13" s="34">
+        <v>15.780000927132599</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="12">
+        <v>9.6525096525096501</v>
+      </c>
+      <c r="C14" s="12">
+        <v>6.5637065637065604</v>
+      </c>
+      <c r="D14" s="12">
+        <v>6.5637065637065604</v>
+      </c>
+      <c r="E14" s="12">
+        <v>6.5637065637065604</v>
+      </c>
+      <c r="F14" s="12">
+        <v>16.8963351106208</v>
+      </c>
+      <c r="G14" s="12">
+        <v>23.279592533384701</v>
+      </c>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="12">
+        <v>13.127413127413099</v>
+      </c>
+      <c r="C15" s="12">
+        <v>10.167310167310101</v>
+      </c>
+      <c r="D15" s="12">
+        <v>10.167310167310101</v>
+      </c>
+      <c r="E15" s="12">
+        <v>10.167310167310101</v>
+      </c>
+      <c r="F15" s="12">
+        <v>22.2683397683397</v>
+      </c>
+      <c r="G15" s="12">
+        <v>29.468833208402401</v>
+      </c>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="14">
+        <v>3.8610038610038599</v>
+      </c>
+      <c r="C16" s="14">
+        <v>2.8314028314028299</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2.8314028314028299</v>
+      </c>
+      <c r="E16" s="14">
+        <v>2.8314028314028299</v>
+      </c>
+      <c r="F16" s="14">
+        <v>6.1733161733161701</v>
+      </c>
+      <c r="G16" s="14">
+        <v>7.6860339551629799</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14">
+        <v>9.6525096525096501</v>
+      </c>
+      <c r="C17" s="14">
+        <v>8.2368082368082298</v>
+      </c>
+      <c r="D17" s="14">
+        <v>8.2368082368082298</v>
+      </c>
+      <c r="E17" s="14">
+        <v>8.2368082368082298</v>
+      </c>
+      <c r="F17" s="14">
+        <v>16.106974321260001</v>
+      </c>
+      <c r="G17" s="14">
+        <v>22.221203970015701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="14">
+        <v>8.8803088803088794</v>
+      </c>
+      <c r="C18" s="14">
+        <v>5.7915057915057897</v>
+      </c>
+      <c r="D18" s="14">
+        <v>5.7915057915057897</v>
+      </c>
+      <c r="E18" s="14">
+        <v>5.7915057915057897</v>
+      </c>
+      <c r="F18" s="14">
+        <v>13.4949745664031</v>
+      </c>
+      <c r="G18" s="14">
+        <v>17.8237076808532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="16">
+        <v>4.6332046332046302</v>
+      </c>
+      <c r="C19" s="16">
+        <v>4.7619047619047601</v>
+      </c>
+      <c r="D19" s="16">
+        <v>4.7619047619047601</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4.7619047619047601</v>
+      </c>
+      <c r="F19" s="16">
+        <v>9.0073236501807905</v>
+      </c>
+      <c r="G19" s="16">
+        <v>12.8070427662543</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="16">
+        <v>6.9498069498069501</v>
+      </c>
+      <c r="C20" s="16">
+        <v>5.7915057915057897</v>
+      </c>
+      <c r="D20" s="16">
+        <v>5.7915057915057897</v>
+      </c>
+      <c r="E20" s="16">
+        <v>5.7915057915057897</v>
+      </c>
+      <c r="F20" s="16">
+        <v>12.3745173745173</v>
+      </c>
+      <c r="G20" s="16">
+        <v>17.281081650700099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="16">
+        <v>11.583011583011499</v>
+      </c>
+      <c r="C21" s="16">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="D21" s="16">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="E21" s="16">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="F21" s="16">
+        <v>17.8553042838757</v>
+      </c>
+      <c r="G21" s="16">
+        <v>23.978196962947901</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="18">
+        <v>0</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0</v>
+      </c>
+      <c r="D22" s="18">
+        <v>0</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0</v>
+      </c>
+      <c r="F22" s="18">
+        <v>0</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B23" s="25">
+        <v>12.3552123552123</v>
+      </c>
+      <c r="C23" s="25">
+        <v>8.2368082368082298</v>
+      </c>
+      <c r="D23" s="25">
+        <v>8.2368082368082298</v>
+      </c>
+      <c r="E23" s="25">
+        <v>8.2368082368082298</v>
+      </c>
+      <c r="F23" s="25">
+        <v>17.882116810688199</v>
+      </c>
+      <c r="G23" s="25">
+        <v>22.638834855528501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="19">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6">
-        <v>9.31</v>
-      </c>
-      <c r="C3" s="6">
-        <v>5.81</v>
-      </c>
-      <c r="D3" s="6">
-        <v>12.98</v>
-      </c>
-      <c r="E3" s="6">
-        <v>7.71</v>
-      </c>
-      <c r="F3" s="6">
-        <v>14.34</v>
-      </c>
-      <c r="G3" s="6">
-        <v>14.94</v>
-      </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7">
-        <v>10.85</v>
-      </c>
-      <c r="C4" s="7">
-        <v>6.72</v>
-      </c>
-      <c r="D4" s="7">
-        <v>15.88</v>
-      </c>
-      <c r="E4" s="7">
-        <v>9.19</v>
-      </c>
-      <c r="F4" s="7">
-        <v>17.510000000000002</v>
-      </c>
-      <c r="G4" s="6">
-        <v>19.309999999999999</v>
-      </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7">
-        <v>5.01</v>
-      </c>
-      <c r="C5" s="7">
-        <v>3.98</v>
-      </c>
-      <c r="D5" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="E5" s="7">
-        <v>5.59</v>
-      </c>
-      <c r="F5" s="7">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="G5" s="6">
-        <v>11.6</v>
-      </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="9">
-        <v>2.3166023166023102</v>
-      </c>
-      <c r="C6" s="9">
-        <v>2.0592020592020499</v>
-      </c>
-      <c r="D6" s="9">
-        <v>2.0592020592020499</v>
-      </c>
-      <c r="E6" s="9">
-        <v>2.0592020592020499</v>
-      </c>
-      <c r="F6" s="9">
-        <v>4.5875467304038704</v>
-      </c>
-      <c r="G6" s="9">
-        <v>6.3742694961931496</v>
-      </c>
-      <c r="H6" s="40">
+      <c r="C24" s="19">
         <v>0</v>
       </c>
-      <c r="I6" s="40">
+      <c r="D24" s="19">
         <v>0</v>
       </c>
-      <c r="J6" s="40">
+      <c r="E24" s="19">
         <v>0</v>
       </c>
-      <c r="K6" s="40">
+      <c r="F24" s="19">
         <v>0</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="9">
-        <v>4.6332046332046302</v>
-      </c>
-      <c r="C7" s="9">
-        <v>4.3758043758043703</v>
-      </c>
-      <c r="D7" s="9">
-        <v>4.3758043758043703</v>
-      </c>
-      <c r="E7" s="9">
-        <v>4.3758043758043703</v>
-      </c>
-      <c r="F7" s="9">
-        <v>9.1829073971931106</v>
-      </c>
-      <c r="G7" s="9">
-        <v>13.7623852619798</v>
-      </c>
-      <c r="H7" s="40">
-        <v>64</v>
-      </c>
-      <c r="I7" s="40">
-        <v>1</v>
-      </c>
-      <c r="J7" s="41">
-        <v>1E-4</v>
-      </c>
-      <c r="K7" s="40">
-        <v>50</v>
-      </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="10">
+      <c r="G24" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="18">
+        <v>0</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0</v>
+      </c>
+      <c r="D25" s="18">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0</v>
+      </c>
+      <c r="F25" s="18">
+        <v>0</v>
+      </c>
+      <c r="G25" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="25">
+        <v>11.583011583011499</v>
+      </c>
+      <c r="C26" s="25">
         <v>7.7220077220077199</v>
       </c>
-      <c r="C8" s="10">
-        <v>6.9498069498069501</v>
-      </c>
-      <c r="D8" s="10">
-        <v>6.9498069498069501</v>
-      </c>
-      <c r="E8" s="10">
-        <v>6.9498069498069501</v>
-      </c>
-      <c r="F8" s="10">
-        <v>15.4283875712447</v>
-      </c>
-      <c r="G8" s="10">
-        <v>22.680937559473801</v>
-      </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="10">
+      <c r="D26" s="25">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="E26" s="25">
+        <v>7.7220077220077199</v>
+      </c>
+      <c r="F26" s="25">
+        <v>16.997916283630499</v>
+      </c>
+      <c r="G26" s="25">
+        <v>21.375786093313099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="25">
         <v>10.8108108108108</v>
       </c>
-      <c r="C9" s="10">
-        <v>7.3359073359073301</v>
-      </c>
-      <c r="D9" s="10">
-        <v>7.3359073359073301</v>
-      </c>
-      <c r="E9" s="10">
-        <v>7.3359073359073301</v>
-      </c>
-      <c r="F9" s="10">
-        <v>17.481154624011701</v>
-      </c>
-      <c r="G9" s="10">
-        <v>23.049457237024701</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1.54440154440154</v>
-      </c>
-      <c r="C10" s="12">
-        <v>2.57400257400257</v>
-      </c>
-      <c r="D10" s="12">
-        <v>2.57400257400257</v>
-      </c>
-      <c r="E10" s="12">
-        <v>2.57400257400257</v>
-      </c>
-      <c r="F10" s="12">
-        <v>5.2253784396641496</v>
-      </c>
-      <c r="G10" s="12">
-        <v>8.5634595960399391</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="12">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="C11" s="12">
-        <v>5.0193050193050199</v>
-      </c>
-      <c r="D11" s="12">
-        <v>5.0193050193050199</v>
-      </c>
-      <c r="E11" s="12">
-        <v>5.0193050193050199</v>
-      </c>
-      <c r="F11" s="12">
-        <v>11.9784580498866</v>
-      </c>
-      <c r="G11" s="12">
-        <v>15.6911707723312</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="12">
-        <v>15.444015444015401</v>
-      </c>
-      <c r="C12" s="12">
-        <v>10.8108108108108</v>
-      </c>
-      <c r="D12" s="12">
-        <v>10.8108108108108</v>
-      </c>
-      <c r="E12" s="12">
-        <v>10.8108108108108</v>
-      </c>
-      <c r="F12" s="12">
-        <v>24.998467855610699</v>
-      </c>
-      <c r="G12" s="20">
-        <v>32.401329519520097</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="20">
-        <v>17.760617760617698</v>
-      </c>
-      <c r="C13" s="20">
-        <v>12.226512226512201</v>
-      </c>
-      <c r="D13" s="20">
-        <v>12.226512226512201</v>
-      </c>
-      <c r="E13" s="20">
-        <v>12.226512226512201</v>
-      </c>
-      <c r="F13" s="20">
-        <v>26.0492124777839</v>
-      </c>
-      <c r="G13" s="12">
-        <v>31.838706064182698</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="35">
-        <v>1.54440154440154</v>
-      </c>
-      <c r="C14" s="35">
-        <v>4.1184041184041096</v>
-      </c>
-      <c r="D14" s="35">
-        <v>4.1184041184041096</v>
-      </c>
-      <c r="E14" s="35">
-        <v>4.1184041184041096</v>
-      </c>
-      <c r="F14" s="35">
-        <v>8.8452227737942</v>
-      </c>
-      <c r="G14" s="35">
-        <v>15.780000927132599</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="14">
-        <v>3.8610038610038599</v>
-      </c>
-      <c r="C15" s="14">
-        <v>2.8314028314028299</v>
-      </c>
-      <c r="D15" s="14">
-        <v>2.8314028314028299</v>
-      </c>
-      <c r="E15" s="14">
-        <v>2.8314028314028299</v>
-      </c>
-      <c r="F15" s="14">
-        <v>6.1733161733161701</v>
-      </c>
-      <c r="G15" s="14">
-        <v>7.6860339551629799</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="14">
-        <v>9.6525096525096501</v>
-      </c>
-      <c r="C16" s="14">
-        <v>8.2368082368082298</v>
-      </c>
-      <c r="D16" s="14">
-        <v>8.2368082368082298</v>
-      </c>
-      <c r="E16" s="14">
-        <v>8.2368082368082298</v>
-      </c>
-      <c r="F16" s="14">
-        <v>16.106974321260001</v>
-      </c>
-      <c r="G16" s="14">
-        <v>22.221203970015701</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="14">
-        <v>8.8803088803088794</v>
-      </c>
-      <c r="C17" s="14">
-        <v>5.7915057915057897</v>
-      </c>
-      <c r="D17" s="14">
-        <v>5.7915057915057897</v>
-      </c>
-      <c r="E17" s="14">
-        <v>5.7915057915057897</v>
-      </c>
-      <c r="F17" s="14">
-        <v>13.4949745664031</v>
-      </c>
-      <c r="G17" s="14">
-        <v>17.8237076808532</v>
-      </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="16">
-        <v>4.6332046332046302</v>
-      </c>
-      <c r="C18" s="16">
-        <v>4.7619047619047601</v>
-      </c>
-      <c r="D18" s="16">
-        <v>4.7619047619047601</v>
-      </c>
-      <c r="E18" s="16">
-        <v>4.7619047619047601</v>
-      </c>
-      <c r="F18" s="16">
-        <v>9.0073236501807905</v>
-      </c>
-      <c r="G18" s="16">
-        <v>12.8070427662543</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="16">
-        <v>6.9498069498069501</v>
-      </c>
-      <c r="C19" s="16">
-        <v>5.7915057915057897</v>
-      </c>
-      <c r="D19" s="16">
-        <v>5.7915057915057897</v>
-      </c>
-      <c r="E19" s="16">
-        <v>5.7915057915057897</v>
-      </c>
-      <c r="F19" s="16">
-        <v>12.3745173745173</v>
-      </c>
-      <c r="G19" s="16">
-        <v>17.281081650700099</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="16">
-        <v>11.583011583011499</v>
-      </c>
-      <c r="C20" s="16">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="D20" s="16">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="E20" s="16">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="F20" s="16">
-        <v>17.8553042838757</v>
-      </c>
-      <c r="G20" s="16">
-        <v>23.978196962947901</v>
-      </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="18">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0</v>
-      </c>
-      <c r="D21" s="18">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <v>0</v>
-      </c>
-      <c r="G21" s="18">
-        <v>0</v>
-      </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="25">
-        <v>12.3552123552123</v>
-      </c>
-      <c r="C22" s="25">
-        <v>8.2368082368082298</v>
-      </c>
-      <c r="D22" s="25">
-        <v>8.2368082368082298</v>
-      </c>
-      <c r="E22" s="25">
-        <v>8.2368082368082298</v>
-      </c>
-      <c r="F22" s="25">
-        <v>17.882116810688199</v>
-      </c>
-      <c r="G22" s="25">
-        <v>22.638834855528501</v>
-      </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="19">
-        <v>0</v>
-      </c>
-      <c r="C23" s="19">
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <v>0</v>
-      </c>
-      <c r="E23" s="19">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19">
-        <v>0</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="18">
-        <v>0</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0</v>
-      </c>
-      <c r="D24" s="18">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="25">
-        <v>11.583011583011499</v>
-      </c>
-      <c r="C25" s="25">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="D25" s="25">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="E25" s="25">
-        <v>7.7220077220077199</v>
-      </c>
-      <c r="F25" s="25">
-        <v>16.997916283630499</v>
-      </c>
-      <c r="G25" s="25">
-        <v>21.375786093313099</v>
-      </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="25">
-        <v>10.8108108108108</v>
-      </c>
-      <c r="C26" s="25">
+      <c r="C27" s="25">
         <v>9.2664092664092603</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D27" s="25">
         <v>9.2664092664092603</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E27" s="25">
         <v>9.2664092664092603</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F27" s="25">
         <v>18.127566341851999</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G27" s="25">
         <v>24.0833954023513</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2072,15 +1875,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">

</xml_diff>